<commit_message>
update yield and fertilizer calculation
</commit_message>
<xml_diff>
--- a/BioSTEAMconnectors/DayCent/user_data.xlsx
+++ b/BioSTEAMconnectors/DayCent/user_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Empli\OneDrive - University of Illinois - Urbana\Documents\GitHub\PythonModule\BioSTEAMconnectors\DayCent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/others/emily/BioSTEAMconnectors/DayCent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FC2FBA-58B7-4576-B119-918693A33084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{E8FC2FBA-58B7-4576-B119-918693A33084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{458DAE36-99D6-4933-9A95-241812A296B9}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="2450" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
   <si>
     <t>CROP_type</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>N_leaching</t>
+  </si>
+  <si>
+    <t>[lbs P/ac]</t>
   </si>
 </sst>
 </file>
@@ -545,23 +548,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.734375" style="7"/>
-    <col min="2" max="7" width="8.734375" style="10"/>
-    <col min="8" max="13" width="8.734375" style="11"/>
-    <col min="14" max="14" width="8.734375" style="10"/>
-    <col min="15" max="15" width="8.734375" style="11"/>
-    <col min="16" max="17" width="8.734375" style="10"/>
-    <col min="18" max="21" width="8.734375" style="11"/>
-    <col min="22" max="16384" width="8.734375" style="7"/>
+    <col min="1" max="1" width="8.7265625" style="7"/>
+    <col min="2" max="7" width="8.7265625" style="10"/>
+    <col min="8" max="13" width="8.7265625" style="11"/>
+    <col min="14" max="14" width="8.7265625" style="10"/>
+    <col min="15" max="15" width="8.7265625" style="11"/>
+    <col min="16" max="17" width="8.7265625" style="10"/>
+    <col min="18" max="21" width="8.7265625" style="11"/>
+    <col min="22" max="16384" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="3">
         <v>0</v>
@@ -624,7 +627,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>21</v>
@@ -687,7 +690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
         <v>13</v>
@@ -720,10 +723,10 @@
         <v>15</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>16</v>
@@ -750,7 +753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>0</v>
       </c>
@@ -762,18 +765,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6238430F-58A6-4A94-8C79-DFABFB8C6037}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.734375" style="7"/>
+    <col min="1" max="16384" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>0</v>
@@ -836,7 +839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -899,7 +902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -932,10 +935,10 @@
         <v>15</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>16</v>
@@ -962,32 +965,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="17" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="18" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="19" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="21" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="22" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="23" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="24" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="25" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="26" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="27" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="28" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="29" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="30" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="31" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="32" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="33" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="34" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="35" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="36" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="37" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>